<commit_message>
Oppdatert med ny info. Semi-fix Ryddet opp uorden
</commit_message>
<xml_diff>
--- a/prosjektplan_msf.xlsx
+++ b/prosjektplan_msf.xlsx
@@ -200,12 +200,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <name val="Arial"/>
@@ -230,8 +224,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,8 +245,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -264,19 +270,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -295,9 +314,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -310,13 +326,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="16" fontId="7" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +652,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H22" sqref="H21:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -639,344 +667,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="21">
         <v>42072</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="21">
         <v>42073</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="20">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="20">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="20">
         <v>2</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="21">
         <v>42072</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="21">
         <v>42073</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="20">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="20">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="21">
         <v>42072</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="21">
         <v>42073</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="20">
         <v>2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="20">
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="20">
         <v>1</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="21">
         <v>42072</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="21">
         <v>42073</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="20">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="20">
         <v>2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="20">
         <v>1</v>
       </c>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="9"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="1"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>42072</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>42072</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>42072</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>42073</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="16">
         <v>42074</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="C20" s="16">
+        <v>42074</v>
+      </c>
+      <c r="D20" s="16">
+        <v>42075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1009,38 +1060,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1072,38 +1123,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1135,38 +1186,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1200,38 +1251,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1262,38 +1313,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1326,38 +1377,38 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
oppdatering av design og info. Fase 1 ferdig
</commit_message>
<xml_diff>
--- a/prosjektplan_msf.xlsx
+++ b/prosjektplan_msf.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>Utvikling av prosjekt X</t>
   </si>
@@ -168,15 +168,6 @@
   </si>
   <si>
     <t>Må revideres i møte nr. 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             2 dager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             3 dager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           1 dag(er)</t>
   </si>
 </sst>
 </file>
@@ -292,7 +283,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -341,6 +332,13 @@
     <xf numFmtId="16" fontId="7" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -651,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H22" sqref="H21:H22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -837,8 +835,8 @@
       <c r="C12" s="16">
         <v>42072</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>46</v>
+      <c r="E12" s="15">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -851,8 +849,8 @@
       <c r="C13" s="16">
         <v>42072</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>46</v>
+      <c r="E13" s="15">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -865,8 +863,8 @@
       <c r="C14" s="16">
         <v>42072</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>47</v>
+      <c r="E14" s="15">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -879,20 +877,33 @@
       <c r="C15" s="16">
         <v>42073</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="E15" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="24">
         <v>42074</v>
       </c>
+      <c r="D16" s="24">
+        <v>42074</v>
+      </c>
+      <c r="E16" s="25">
+        <v>2</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+      <c r="G16" s="18">
+        <v>1</v>
+      </c>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
@@ -911,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20" s="16">
         <v>42074</v>
@@ -1024,9 +1035,18 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="E38" s="4">
+        <f>E5+E6+E8+E9+E13+E12+E14+E15+E16+E20+E21+E22+E23+E24+E27+E28+E29+E30+E33+E34+E35+E36+E37</f>
+        <v>64</v>
+      </c>
+      <c r="F38" s="4">
+        <f>F5+F6+F8+F9+F12+F13+F14+F15+F16+F20+F21+F22+F23+F24+F26+F27+F28+F29+F30+F31+F32+F33+F34+F36+F35+F37</f>
+        <v>12</v>
+      </c>
+      <c r="G38" s="4">
+        <f>G5+G6+G8+G9+G12+G13+G14+G15+G16+G20+G21+G22+G23+G24+G25+G27+G28+G29+G30+G33+G34+G35+G36+G37</f>
+        <v>5</v>
+      </c>
       <c r="H38" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oppdaterte roller. Systematisert penere
</commit_message>
<xml_diff>
--- a/prosjektplan_msf.xlsx
+++ b/prosjektplan_msf.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>Utvikling av prosjekt X</t>
   </si>
@@ -155,26 +155,77 @@
     <t>Tanja</t>
   </si>
   <si>
-    <t>Tobias</t>
+    <t>Felles</t>
+  </si>
+  <si>
+    <t>Må revideres i møte nr. 2</t>
+  </si>
+  <si>
+    <t>neste iterasjon</t>
+  </si>
+  <si>
+    <t>Enighet har blitt gjort</t>
+  </si>
+  <si>
+    <t>Tobias/Tanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Må: Samkjøre design. Fikse kanter. Stilrent. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Må ryddes opp. </t>
+  </si>
+  <si>
+    <t>Oppdaterte sannsynligheter basert på efaringer i løpet av uken</t>
+  </si>
+  <si>
+    <t>Eirikur/Iben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tobias/Iben </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eirikur/Iben </t>
+  </si>
+  <si>
+    <t>Utviklere</t>
   </si>
   <si>
     <t>Eirikur</t>
   </si>
   <si>
-    <t>Felles</t>
-  </si>
-  <si>
-    <t>Endring i formulering</t>
-  </si>
-  <si>
-    <t>Må revideres i møte nr. 2</t>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Fungerer optimalt lokalt. Må flyttes til hoved-server for videre testing. (Home.nith.no)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>Generell opplæring av ny kunnskap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ny kunnskap var nødvendig for prosjektet. </t>
+  </si>
+  <si>
+    <t>F.A.Q implementert. Skal legges til i løsningen</t>
+  </si>
+  <si>
+    <t>Utrulling har og vil alltid være aktivt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-414]d/\ mmm\.;@"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -211,19 +262,58 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,11 +328,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -263,35 +373,85 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -318,33 +478,67 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="16" fontId="7" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="16" fontId="9" fillId="6" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="7"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+  <cellStyles count="9">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="7" builtinId="22"/>
+    <cellStyle name="Explanatory Text" xfId="8" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -665,389 +859,660 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>42072</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="18">
         <v>42073</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="16">
         <v>5</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="16">
         <v>3</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="16">
+        <f>E5-F5</f>
         <v>2</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D6" s="18">
+        <v>42073</v>
+      </c>
+      <c r="E6" s="16">
+        <v>3</v>
+      </c>
+      <c r="F6" s="16">
+        <v>3</v>
+      </c>
+      <c r="G6" s="16">
+        <f>E6-F6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D8" s="18">
+        <v>42073</v>
+      </c>
+      <c r="E8" s="16">
+        <v>2</v>
+      </c>
+      <c r="F8" s="16">
+        <v>3</v>
+      </c>
+      <c r="G8" s="16">
+        <f>E8-F8</f>
+        <v>-1</v>
+      </c>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D9" s="18">
+        <v>42073</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16">
+        <f>E9-F9</f>
+        <v>-1</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D10" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E10" s="29">
+        <v>10</v>
+      </c>
+      <c r="F10" s="29">
+        <v>8</v>
+      </c>
+      <c r="G10" s="29">
+        <f>E10-F10</f>
+        <v>2</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="18">
+        <v>42074</v>
+      </c>
+      <c r="D13" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E13" s="16">
+        <v>10</v>
+      </c>
+      <c r="G13" s="16">
+        <f>E13-F13</f>
+        <v>10</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D14" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E14" s="16">
+        <v>12</v>
+      </c>
+      <c r="F14" s="16">
+        <v>12</v>
+      </c>
+      <c r="G14" s="16">
+        <f t="shared" ref="G14:G37" si="0">E14-F14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="22" t="s">
+      <c r="C15" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D15" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E15" s="16">
+        <v>15</v>
+      </c>
+      <c r="F15" s="16">
+        <v>25</v>
+      </c>
+      <c r="G15" s="16">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="18">
+        <v>42073</v>
+      </c>
+      <c r="D16" s="25">
+        <v>42076</v>
+      </c>
+      <c r="E16" s="16">
+        <v>8</v>
+      </c>
+      <c r="G16" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C17" s="18">
+        <v>42074</v>
+      </c>
+      <c r="D17" s="18">
+        <v>42074</v>
+      </c>
+      <c r="E17" s="21">
+        <v>2</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="18">
+        <v>42074</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E21" s="16">
+        <v>3</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="18">
+        <v>42073</v>
+      </c>
+      <c r="D22" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E22" s="16">
+        <v>10</v>
+      </c>
+      <c r="F22" s="16">
+        <v>7</v>
+      </c>
+      <c r="G22" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="18">
+        <v>42074</v>
+      </c>
+      <c r="D23" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E23" s="16">
+        <v>7</v>
+      </c>
+      <c r="F23" s="16">
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="18">
+        <v>42075</v>
+      </c>
+      <c r="D24" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E24" s="38">
+        <v>3</v>
+      </c>
+      <c r="F24" s="37">
+        <v>2</v>
+      </c>
+      <c r="G24" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E25" s="39">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="18">
+        <v>42075</v>
+      </c>
+      <c r="D29" s="18">
+        <v>42075</v>
+      </c>
+      <c r="E29" s="16">
+        <v>5</v>
+      </c>
+      <c r="F29" s="16">
+        <v>3</v>
+      </c>
+      <c r="G29" s="16">
+        <f>E29-F29</f>
+        <v>2</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="13">
+        <v>42076</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <f>E30-F30</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24">
+        <f>E31-F31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24">
+        <f>E32-F32</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <f>E33-F33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="G35">
+        <f>E35-F35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36">
+        <f>E36-F36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="18">
         <v>42072</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D37" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="31"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14">
+        <f>E37-F37</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="18">
+        <v>42072</v>
+      </c>
+      <c r="D38" s="18">
         <v>42073</v>
       </c>
-      <c r="E6" s="20">
-        <v>3</v>
-      </c>
-      <c r="F6" s="20">
-        <v>3</v>
-      </c>
-      <c r="G6" s="20">
+      <c r="E38" s="16">
+        <v>2</v>
+      </c>
+      <c r="F38" s="16">
+        <v>1</v>
+      </c>
+      <c r="G38" s="16">
+        <f>E38-F38</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <f>E39-F39</f>
         <v>0</v>
       </c>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="21">
-        <v>42072</v>
-      </c>
-      <c r="D8" s="21">
-        <v>42073</v>
-      </c>
-      <c r="E8" s="20">
-        <v>2</v>
-      </c>
-      <c r="F8" s="20">
-        <v>3</v>
-      </c>
-      <c r="G8" s="20">
+    </row>
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="18">
+        <v>42075</v>
+      </c>
+      <c r="D40" s="32"/>
+      <c r="E40" s="33">
         <v>1</v>
       </c>
-      <c r="H8" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="21">
-        <v>42072</v>
-      </c>
-      <c r="D9" s="21">
-        <v>42073</v>
-      </c>
-      <c r="E9" s="20">
-        <v>1</v>
-      </c>
-      <c r="F9" s="20">
-        <v>2</v>
-      </c>
-      <c r="G9" s="20">
-        <v>1</v>
-      </c>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="16">
-        <v>42072</v>
-      </c>
-      <c r="E12" s="15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="16">
-        <v>42072</v>
-      </c>
-      <c r="E13" s="15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26">
+        <f>E5+E6+E8+E9+E10+E14+E13+E15+E16+E17+E21+E22+E23+E24+E25+E29+E30+E31+E32+E36+E37+E38+E39+E40</f>
+        <v>105</v>
+      </c>
+      <c r="F41" s="26">
+        <f>F5+F6+F8+F9+F10+F13+F14+F15+F16+F17+F21+F22+F23+F24+F25+F28+F29+F30+F31+F32+F33+F35+F36+F37+F39+F38+F40</f>
+        <v>75</v>
+      </c>
+      <c r="G41" s="26">
+        <f>G5+G6+G8+G9+G10+G13+G14+G15+G16+G17+G21+G22+G23+G24+G25+G26+G29+G30+G31+G32+G36+G37+G38+G39+G40</f>
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="16">
-        <v>42072</v>
-      </c>
-      <c r="E14" s="15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="16">
-        <v>42073</v>
-      </c>
-      <c r="E15" s="15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="24">
-        <v>42074</v>
-      </c>
-      <c r="D16" s="24">
-        <v>42074</v>
-      </c>
-      <c r="E16" s="25">
-        <v>2</v>
-      </c>
-      <c r="F16" s="18">
-        <v>1</v>
-      </c>
-      <c r="G16" s="18">
-        <v>1</v>
-      </c>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="16">
-        <v>42074</v>
-      </c>
-      <c r="D20" s="16">
-        <v>42075</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4">
-        <f>E5+E6+E8+E9+E13+E12+E14+E15+E16+E20+E21+E22+E23+E24+E27+E28+E29+E30+E33+E34+E35+E36+E37</f>
-        <v>64</v>
-      </c>
-      <c r="F38" s="4">
-        <f>F5+F6+F8+F9+F12+F13+F14+F15+F16+F20+F21+F22+F23+F24+F26+F27+F28+F29+F30+F31+F32+F33+F34+F36+F35+F37</f>
-        <v>12</v>
-      </c>
-      <c r="G38" s="4">
-        <f>G5+G6+G8+G9+G12+G13+G14+G15+G16+G20+G21+G22+G23+G24+G25+G27+G28+G29+G30+G33+G34+G35+G36+G37</f>
-        <v>5</v>
-      </c>
-      <c r="H38" s="4"/>
+      <c r="H41" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1080,38 +1545,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1143,38 +1608,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1206,38 +1671,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1271,38 +1736,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1333,38 +1798,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1397,38 +1862,38 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>